<commit_message>
update analogue, geochem and geo-energy vocab source files
</commit_message>
<xml_diff>
--- a/storage/app/keywords/1-3/240418 MSL vocabulary Geochemistry.xlsx
+++ b/storage/app/keywords/1-3/240418 MSL vocabulary Geochemistry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28602"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/r_p_j_pijnenburg_uu_nl/Documents/EPOS-NL/07 Data/Metadata/240219 MSL vocabs 1.2 - update not yet implemented/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{BB62AF8B-DD80-4EB3-96A2-8B81BA299D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{511917CF-3904-4F92-B41F-7979D74459C7}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{BB62AF8B-DD80-4EB3-96A2-8B81BA299D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EAD6F70-8A86-4271-A8A1-8BD661CDE817}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -545,7 +545,7 @@
     <t>x-ray fluorescence spectrometer</t>
   </si>
   <si>
-    <t>#xrf</t>
+    <t>#xrf #(XRF) #X-ray fluorescence #X-ray fluoresence</t>
   </si>
   <si>
     <t>https://epos-msl.uu.nl/voc/geochemistry/1.2/technique-x-ray_spectrometry-x-ray_fluorescence</t>
@@ -2473,7 +2473,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -2484,6 +2484,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2792,15 +2795,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H319"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="6"/>
     <col min="2" max="4" width="32" style="6" customWidth="1"/>
-    <col min="5" max="8" width="8.7109375" style="6"/>
+    <col min="5" max="5" width="36.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="8.7109375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3900,11 +3904,11 @@
         <v>167</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" ht="30.75">
       <c r="C91" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="E91" s="6" t="s">
+      <c r="E91" s="9" t="s">
         <v>169</v>
       </c>
       <c r="F91" s="6" t="s">
@@ -6400,26 +6404,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="53df6a5f-9334-4503-a845-5e05459a4c71" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2184524c-f8db-481f-81f4-afb1a4d0a68c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ED960ACB7111C64DB882066D7ADB6F8C" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fc52296ac513abf3bf0c805f47d07abe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2184524c-f8db-481f-81f4-afb1a4d0a68c" xmlns:ns3="53df6a5f-9334-4503-a845-5e05459a4c71" xmlns:ns4="6965ef5a-98c2-4976-9e1e-bc6458d0e33d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8080ad1dda7eb37606acae043215b69b" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="2184524c-f8db-481f-81f4-afb1a4d0a68c"/>
@@ -6673,8 +6657,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="53df6a5f-9334-4503-a845-5e05459a4c71" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2184524c-f8db-481f-81f4-afb1a4d0a68c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68D2101F-89E1-4E37-AD9C-48EE9788084E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B244D19-2F79-4EB5-9BAC-241FD40E5C0C}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6682,5 +6686,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B244D19-2F79-4EB5-9BAC-241FD40E5C0C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68D2101F-89E1-4E37-AD9C-48EE9788084E}"/>
 </file>
</xml_diff>